<commit_message>
Updated a few files and added a function in the Plotting.jl module that will plot species on demand
</commit_message>
<xml_diff>
--- a/IMPORTANT_RXN_COLORS.xlsx
+++ b/IMPORTANT_RXN_COLORS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t xml:space="preserve">Color</t>
   </si>
@@ -35,151 +35,145 @@
     <t xml:space="preserve">D reaction</t>
   </si>
   <si>
+    <t xml:space="preserve">#e23209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#891E06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCOpl + E --&gt; CO + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCOpl + E --&gt; CO + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#44AA99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#2F7569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2pl + H2 --&gt; HCO2pl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2pl + HD --&gt; HCO2pl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9867f6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#117733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#083617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opl + H2 --&gt; OHpl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opl + HD --&gt; OHpl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ae6529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#999933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#5C5C1F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCO2pl + E --&gt; CO + O + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCO2pl + E --&gt; CO + O + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#598322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#CC6677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#A8384B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OHpl + O --&gt; O2pl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODpl + O --&gt; O2pl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#3f1ba1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#882255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#521433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2pl + H2 --&gt; N2Hpl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2pl + HD --&gt; N2Hpl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#7e2640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#57b230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2pl + CO2 --&gt; HCO2pl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDpl + CO2 --&gt; HCO2pl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#453cc5</t>
+  </si>
+  <si>
     <t xml:space="preserve">#332288</t>
   </si>
   <si>
     <t xml:space="preserve">#1F1452</t>
   </si>
   <si>
-    <t xml:space="preserve">HCOpl + E --&gt; CO + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCOpl + E --&gt; CO + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#e23209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#44AA99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#2F7569</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2pl + H2 --&gt; HCO2pl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2pl + HD --&gt; HCO2pl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#9867f6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#117733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#083617</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opl + H2 --&gt; OHpl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opl + HD --&gt; OHpl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#ae6529</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#999933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#5C5C1F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCO2pl + E --&gt; CO + O + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCO2pl + E --&gt; CO + O + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#598322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#CC6677</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#A8384B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OHpl + O --&gt; O2pl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODpl + O --&gt; O2pl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#3f1ba1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#882255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#521433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2pl + H2 --&gt; N2Hpl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2pl + HD --&gt; N2Hpl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#7e2640</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#57b230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2pl + CO2 --&gt; HCO2pl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDpl + CO2 --&gt; HCO2pl + D</t>
+    <t xml:space="preserve">Hpl + H --&gt; H + Hpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dpl + H --&gt; D + Hpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#056e12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OHpl + H2 --&gt; H2Opl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OHpl + HD --&gt; H2Opl + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ea88e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OHpl + E --&gt; O + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODpl + E --&gt; O + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ee983a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2pl + O --&gt; OHpl + H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDpl + O --&gt; OHpl + D</t>
   </si>
   <si>
     <t xml:space="preserve">#bf11af</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 --&gt; H + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HD --&gt; H + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#056e12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OHpl + H2 --&gt; H2Opl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OHpl + HD --&gt; H2Opl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#ea88e2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OHpl + E --&gt; O + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODpl + E --&gt; O + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#28412c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hpl + H --&gt; H + Hpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dpl + H --&gt; D + Hpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#ee983a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2pl + O --&gt; OHpl + H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDpl + O --&gt; OHpl + D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#453cc5</t>
   </si>
   <si>
     <t xml:space="preserve">Hpl + O2 --&gt; O2pl + H</t>
@@ -364,12 +358,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -389,13 +383,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="27.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.79"/>
@@ -419,7 +413,7 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -428,247 +422,278 @@
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -690,10 +715,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.08"/>
@@ -712,69 +737,69 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>